<commit_message>
Alternate form factor work
</commit_message>
<xml_diff>
--- a/mini_rev0/aqplus_mini_rev0_CPL1.xlsx
+++ b/mini_rev0/aqplus_mini_rev0_CPL1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\System\pcb\mini_rev0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7389E2FA-6C50-4785-8483-F3FD8B3FCF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC10E06-7087-4178-9BA6-F5D0B7996097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1278,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,7 +2163,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>75.5</v>
+        <v>76.77</v>
       </c>
       <c r="C52">
         <v>-122.175</v>
@@ -2183,7 +2183,7 @@
         <v>77.467151999999999</v>
       </c>
       <c r="C53">
-        <v>-44.459468999999999</v>
+        <v>-45.8</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
@@ -2197,16 +2197,16 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>101</v>
+        <v>97.45</v>
       </c>
       <c r="C54">
-        <v>-53.86</v>
+        <v>-52.5</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>119</v>
       </c>
       <c r="C55">
-        <v>-48</v>
+        <v>-48.65</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
@@ -2231,10 +2231,10 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>149</v>
+        <v>149.19999999999999</v>
       </c>
       <c r="C56">
-        <v>-43</v>
+        <v>-54.5</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
@@ -2251,7 +2251,7 @@
         <v>96</v>
       </c>
       <c r="C57">
-        <v>-98.67</v>
+        <v>-109.02</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
@@ -2302,7 +2302,7 @@
         <v>75.674599999999998</v>
       </c>
       <c r="C60">
-        <v>-56.525399999999998</v>
+        <v>-55.25</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
@@ -2319,7 +2319,7 @@
         <v>79.914599999999993</v>
       </c>
       <c r="C61">
-        <v>-56.525399999999998</v>
+        <v>-55.25</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
@@ -2333,7 +2333,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>84.804199999999994</v>
+        <v>86.05</v>
       </c>
       <c r="C62">
         <v>-66.007000000000005</v>

</xml_diff>